<commit_message>
Add main.cpp test file, rework Excel test file
</commit_message>
<xml_diff>
--- a/test/test_spreadsheet.xlsx
+++ b/test/test_spreadsheet.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t xml:space="preserve">Param name 1</t>
   </si>
@@ -217,10 +217,10 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.43"/>
@@ -360,8 +360,8 @@
       <c r="D4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="0" t="n">
-        <v>3</v>
+      <c r="E4" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>3</v>
@@ -395,6 +395,12 @@
       <c r="C5" s="0" t="s">
         <v>25</v>
       </c>
+      <c r="D5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>26</v>
+      </c>
       <c r="I5" s="0" t="n">
         <v>4</v>
       </c>
@@ -427,6 +433,12 @@
       <c r="C6" s="0" t="s">
         <v>28</v>
       </c>
+      <c r="D6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>26</v>
+      </c>
       <c r="I6" s="0" t="n">
         <v>5</v>
       </c>
@@ -458,6 +470,12 @@
       </c>
       <c r="C7" s="0" t="s">
         <v>31</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>6</v>
@@ -504,7 +522,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="str">

</xml_diff>